<commit_message>
Fixing component errors; Q1 is an SOT-23 not an SC-70, some components were out of stock, had wrong attributes, etc. BOM is now mostly error free.
</commit_message>
<xml_diff>
--- a/1u_panel/1u_panel.xlsx
+++ b/1u_panel/1u_panel.xlsx
@@ -166,14 +166,11 @@
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
@@ -188,10 +185,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:IQ83"/>
+  <dimension ref="A1:IP83"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="F42" sqref="F42"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -269,10 +266,10 @@
     <col min="248" max="248" style="0" width="8.14236778846154" bestFit="1" customWidth="1"/>
     <col min="249" max="249" style="0" width="11.85643028846154" bestFit="1" customWidth="1"/>
     <col min="250" max="250" style="0" width="8.71376201923077" bestFit="1" customWidth="1"/>
-    <col min="251" max="256" style="0" width="9.142307692307693"/>
+    <col min="251" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:251">
+    <row r="1" spans="1:250">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Bill Of Materials for OreSat Solar Module</t>
@@ -287,7 +284,6 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-      <c r="K1" s="2"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -297,7 +293,6 @@
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
-      <c r="U1" s="2"/>
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
       <c r="X1" s="1"/>
@@ -307,7 +302,6 @@
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
-      <c r="AE1" s="2"/>
       <c r="AF1" s="1"/>
       <c r="AG1" s="1"/>
       <c r="AH1" s="1"/>
@@ -317,7 +311,6 @@
       <c r="AL1" s="1"/>
       <c r="AM1" s="1"/>
       <c r="AN1" s="1"/>
-      <c r="AO1" s="2"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
       <c r="AR1" s="1"/>
@@ -327,7 +320,6 @@
       <c r="AV1" s="1"/>
       <c r="AW1" s="1"/>
       <c r="AX1" s="1"/>
-      <c r="AY1" s="2"/>
       <c r="AZ1" s="1"/>
       <c r="BA1" s="1"/>
       <c r="BB1" s="1"/>
@@ -337,7 +329,6 @@
       <c r="BF1" s="1"/>
       <c r="BG1" s="1"/>
       <c r="BH1" s="1"/>
-      <c r="BI1" s="2"/>
       <c r="BJ1" s="1"/>
       <c r="BK1" s="1"/>
       <c r="BL1" s="1"/>
@@ -347,7 +338,6 @@
       <c r="BP1" s="1"/>
       <c r="BQ1" s="1"/>
       <c r="BR1" s="1"/>
-      <c r="BS1" s="2"/>
       <c r="BT1" s="1"/>
       <c r="BU1" s="1"/>
       <c r="BV1" s="1"/>
@@ -357,7 +347,6 @@
       <c r="BZ1" s="1"/>
       <c r="CA1" s="1"/>
       <c r="CB1" s="1"/>
-      <c r="CC1" s="2"/>
       <c r="CD1" s="1"/>
       <c r="CE1" s="1"/>
       <c r="CF1" s="1"/>
@@ -367,7 +356,6 @@
       <c r="CJ1" s="1"/>
       <c r="CK1" s="1"/>
       <c r="CL1" s="1"/>
-      <c r="CM1" s="2"/>
       <c r="CN1" s="1"/>
       <c r="CO1" s="1"/>
       <c r="CP1" s="1"/>
@@ -377,7 +365,6 @@
       <c r="CT1" s="1"/>
       <c r="CU1" s="1"/>
       <c r="CV1" s="1"/>
-      <c r="CW1" s="2"/>
       <c r="CX1" s="1"/>
       <c r="CY1" s="1"/>
       <c r="CZ1" s="1"/>
@@ -387,7 +374,6 @@
       <c r="DD1" s="1"/>
       <c r="DE1" s="1"/>
       <c r="DF1" s="1"/>
-      <c r="DG1" s="2"/>
       <c r="DH1" s="1"/>
       <c r="DI1" s="1"/>
       <c r="DJ1" s="1"/>
@@ -397,7 +383,6 @@
       <c r="DN1" s="1"/>
       <c r="DO1" s="1"/>
       <c r="DP1" s="1"/>
-      <c r="DQ1" s="2"/>
       <c r="DR1" s="1"/>
       <c r="DS1" s="1"/>
       <c r="DT1" s="1"/>
@@ -407,7 +392,6 @@
       <c r="DX1" s="1"/>
       <c r="DY1" s="1"/>
       <c r="DZ1" s="1"/>
-      <c r="EA1" s="2"/>
       <c r="EB1" s="1"/>
       <c r="EC1" s="1"/>
       <c r="ED1" s="1"/>
@@ -417,7 +401,6 @@
       <c r="EH1" s="1"/>
       <c r="EI1" s="1"/>
       <c r="EJ1" s="1"/>
-      <c r="EK1" s="2"/>
       <c r="EL1" s="1"/>
       <c r="EM1" s="1"/>
       <c r="EN1" s="1"/>
@@ -427,7 +410,6 @@
       <c r="ER1" s="1"/>
       <c r="ES1" s="1"/>
       <c r="ET1" s="1"/>
-      <c r="EU1" s="2"/>
       <c r="EV1" s="1"/>
       <c r="EW1" s="1"/>
       <c r="EX1" s="1"/>
@@ -437,7 +419,6 @@
       <c r="FB1" s="1"/>
       <c r="FC1" s="1"/>
       <c r="FD1" s="1"/>
-      <c r="FE1" s="2"/>
       <c r="FF1" s="1"/>
       <c r="FG1" s="1"/>
       <c r="FH1" s="1"/>
@@ -447,7 +428,6 @@
       <c r="FL1" s="1"/>
       <c r="FM1" s="1"/>
       <c r="FN1" s="1"/>
-      <c r="FO1" s="2"/>
       <c r="FP1" s="1"/>
       <c r="FQ1" s="1"/>
       <c r="FR1" s="1"/>
@@ -457,7 +437,6 @@
       <c r="FV1" s="1"/>
       <c r="FW1" s="1"/>
       <c r="FX1" s="1"/>
-      <c r="FY1" s="2"/>
       <c r="FZ1" s="1"/>
       <c r="GA1" s="1"/>
       <c r="GB1" s="1"/>
@@ -467,7 +446,6 @@
       <c r="GF1" s="1"/>
       <c r="GG1" s="1"/>
       <c r="GH1" s="1"/>
-      <c r="GI1" s="2"/>
       <c r="GJ1" s="1" t="s">
         <v>0</v>
       </c>
@@ -479,7 +457,6 @@
       <c r="GP1" s="1"/>
       <c r="GQ1" s="1"/>
       <c r="GR1" s="1"/>
-      <c r="GS1" s="2"/>
       <c r="GT1" s="1" t="s">
         <v>0</v>
       </c>
@@ -491,7 +468,6 @@
       <c r="GZ1" s="1"/>
       <c r="HA1" s="1"/>
       <c r="HB1" s="1"/>
-      <c r="HC1" s="2"/>
       <c r="HD1" s="1" t="s">
         <v>0</v>
       </c>
@@ -503,7 +479,6 @@
       <c r="HJ1" s="1"/>
       <c r="HK1" s="1"/>
       <c r="HL1" s="1"/>
-      <c r="HM1" s="2"/>
       <c r="HN1" s="1" t="s">
         <v>0</v>
       </c>
@@ -515,7 +490,6 @@
       <c r="HT1" s="1"/>
       <c r="HU1" s="1"/>
       <c r="HV1" s="1"/>
-      <c r="HW1" s="2"/>
       <c r="HX1" s="1" t="s">
         <v>0</v>
       </c>
@@ -527,7 +501,6 @@
       <c r="ID1" s="1"/>
       <c r="IE1" s="1"/>
       <c r="IF1" s="1"/>
-      <c r="IG1" s="2"/>
       <c r="IH1" s="1" t="s">
         <v>0</v>
       </c>
@@ -539,9 +512,8 @@
       <c r="IN1" s="1"/>
       <c r="IO1" s="1"/>
       <c r="IP1" s="1"/>
-      <c r="IQ1" s="2"/>
-    </row>
-    <row r="2" spans="1:251">
+    </row>
+    <row r="2" spans="1:250">
       <c r="A2" s="1" t="inlineStr">
         <is>
           <t>source file: 1u_panel.sch</t>
@@ -553,190 +525,152 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="2"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="2"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
-      <c r="R2" s="2"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
-      <c r="U2" s="2"/>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
-      <c r="AB2" s="2"/>
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
-      <c r="AE2" s="2"/>
       <c r="AF2" s="1"/>
       <c r="AG2" s="1"/>
       <c r="AH2" s="1"/>
       <c r="AI2" s="1"/>
       <c r="AJ2" s="1"/>
       <c r="AK2" s="1"/>
-      <c r="AL2" s="2"/>
       <c r="AM2" s="1"/>
       <c r="AN2" s="1"/>
-      <c r="AO2" s="2"/>
       <c r="AP2" s="1"/>
       <c r="AQ2" s="1"/>
       <c r="AR2" s="1"/>
       <c r="AS2" s="1"/>
       <c r="AT2" s="1"/>
       <c r="AU2" s="1"/>
-      <c r="AV2" s="2"/>
       <c r="AW2" s="1"/>
       <c r="AX2" s="1"/>
-      <c r="AY2" s="2"/>
       <c r="AZ2" s="1"/>
       <c r="BA2" s="1"/>
       <c r="BB2" s="1"/>
       <c r="BC2" s="1"/>
       <c r="BD2" s="1"/>
       <c r="BE2" s="1"/>
-      <c r="BF2" s="2"/>
       <c r="BG2" s="1"/>
       <c r="BH2" s="1"/>
-      <c r="BI2" s="2"/>
       <c r="BJ2" s="1"/>
       <c r="BK2" s="1"/>
       <c r="BL2" s="1"/>
       <c r="BM2" s="1"/>
       <c r="BN2" s="1"/>
       <c r="BO2" s="1"/>
-      <c r="BP2" s="2"/>
       <c r="BQ2" s="1"/>
       <c r="BR2" s="1"/>
-      <c r="BS2" s="2"/>
       <c r="BT2" s="1"/>
       <c r="BU2" s="1"/>
       <c r="BV2" s="1"/>
       <c r="BW2" s="1"/>
       <c r="BX2" s="1"/>
       <c r="BY2" s="1"/>
-      <c r="BZ2" s="2"/>
       <c r="CA2" s="1"/>
       <c r="CB2" s="1"/>
-      <c r="CC2" s="2"/>
       <c r="CD2" s="1"/>
       <c r="CE2" s="1"/>
       <c r="CF2" s="1"/>
       <c r="CG2" s="1"/>
       <c r="CH2" s="1"/>
       <c r="CI2" s="1"/>
-      <c r="CJ2" s="2"/>
       <c r="CK2" s="1"/>
       <c r="CL2" s="1"/>
-      <c r="CM2" s="2"/>
       <c r="CN2" s="1"/>
       <c r="CO2" s="1"/>
       <c r="CP2" s="1"/>
       <c r="CQ2" s="1"/>
       <c r="CR2" s="1"/>
       <c r="CS2" s="1"/>
-      <c r="CT2" s="2"/>
       <c r="CU2" s="1"/>
       <c r="CV2" s="1"/>
-      <c r="CW2" s="2"/>
       <c r="CX2" s="1"/>
       <c r="CY2" s="1"/>
       <c r="CZ2" s="1"/>
       <c r="DA2" s="1"/>
       <c r="DB2" s="1"/>
       <c r="DC2" s="1"/>
-      <c r="DD2" s="2"/>
       <c r="DE2" s="1"/>
       <c r="DF2" s="1"/>
-      <c r="DG2" s="2"/>
       <c r="DH2" s="1"/>
       <c r="DI2" s="1"/>
       <c r="DJ2" s="1"/>
       <c r="DK2" s="1"/>
       <c r="DL2" s="1"/>
       <c r="DM2" s="1"/>
-      <c r="DN2" s="2"/>
       <c r="DO2" s="1"/>
       <c r="DP2" s="1"/>
-      <c r="DQ2" s="2"/>
       <c r="DR2" s="1"/>
       <c r="DS2" s="1"/>
       <c r="DT2" s="1"/>
       <c r="DU2" s="1"/>
       <c r="DV2" s="1"/>
       <c r="DW2" s="1"/>
-      <c r="DX2" s="2"/>
       <c r="DY2" s="1"/>
       <c r="DZ2" s="1"/>
-      <c r="EA2" s="2"/>
       <c r="EB2" s="1"/>
       <c r="EC2" s="1"/>
       <c r="ED2" s="1"/>
       <c r="EE2" s="1"/>
       <c r="EF2" s="1"/>
       <c r="EG2" s="1"/>
-      <c r="EH2" s="2"/>
       <c r="EI2" s="1"/>
       <c r="EJ2" s="1"/>
-      <c r="EK2" s="2"/>
       <c r="EL2" s="1"/>
       <c r="EM2" s="1"/>
       <c r="EN2" s="1"/>
       <c r="EO2" s="1"/>
       <c r="EP2" s="1"/>
       <c r="EQ2" s="1"/>
-      <c r="ER2" s="2"/>
       <c r="ES2" s="1"/>
       <c r="ET2" s="1"/>
-      <c r="EU2" s="2"/>
       <c r="EV2" s="1"/>
       <c r="EW2" s="1"/>
       <c r="EX2" s="1"/>
       <c r="EY2" s="1"/>
       <c r="EZ2" s="1"/>
       <c r="FA2" s="1"/>
-      <c r="FB2" s="2"/>
       <c r="FC2" s="1"/>
       <c r="FD2" s="1"/>
-      <c r="FE2" s="2"/>
       <c r="FF2" s="1"/>
       <c r="FG2" s="1"/>
       <c r="FH2" s="1"/>
       <c r="FI2" s="1"/>
       <c r="FJ2" s="1"/>
       <c r="FK2" s="1"/>
-      <c r="FL2" s="2"/>
       <c r="FM2" s="1"/>
       <c r="FN2" s="1"/>
-      <c r="FO2" s="2"/>
       <c r="FP2" s="1"/>
       <c r="FQ2" s="1"/>
       <c r="FR2" s="1"/>
       <c r="FS2" s="1"/>
       <c r="FT2" s="1"/>
       <c r="FU2" s="1"/>
-      <c r="FV2" s="2"/>
       <c r="FW2" s="1"/>
       <c r="FX2" s="1"/>
-      <c r="FY2" s="2"/>
       <c r="FZ2" s="1"/>
       <c r="GA2" s="1"/>
       <c r="GB2" s="1"/>
       <c r="GC2" s="1"/>
       <c r="GD2" s="1"/>
       <c r="GE2" s="1"/>
-      <c r="GF2" s="2"/>
       <c r="GG2" s="1"/>
       <c r="GH2" s="1"/>
-      <c r="GI2" s="2"/>
       <c r="GJ2" s="1" t="s">
         <v>1</v>
       </c>
@@ -745,10 +679,8 @@
       <c r="GM2" s="1"/>
       <c r="GN2" s="1"/>
       <c r="GO2" s="1"/>
-      <c r="GP2" s="2"/>
       <c r="GQ2" s="1"/>
       <c r="GR2" s="1"/>
-      <c r="GS2" s="2"/>
       <c r="GT2" s="1" t="s">
         <v>1</v>
       </c>
@@ -757,10 +689,8 @@
       <c r="GW2" s="1"/>
       <c r="GX2" s="1"/>
       <c r="GY2" s="1"/>
-      <c r="GZ2" s="2"/>
       <c r="HA2" s="1"/>
       <c r="HB2" s="1"/>
-      <c r="HC2" s="2"/>
       <c r="HD2" s="1" t="s">
         <v>1</v>
       </c>
@@ -769,10 +699,8 @@
       <c r="HG2" s="1"/>
       <c r="HH2" s="1"/>
       <c r="HI2" s="1"/>
-      <c r="HJ2" s="2"/>
       <c r="HK2" s="1"/>
       <c r="HL2" s="1"/>
-      <c r="HM2" s="2"/>
       <c r="HN2" s="1" t="s">
         <v>1</v>
       </c>
@@ -781,10 +709,8 @@
       <c r="HQ2" s="1"/>
       <c r="HR2" s="1"/>
       <c r="HS2" s="1"/>
-      <c r="HT2" s="2"/>
       <c r="HU2" s="1"/>
       <c r="HV2" s="1"/>
-      <c r="HW2" s="2"/>
       <c r="HX2" s="1" t="s">
         <v>1</v>
       </c>
@@ -793,10 +719,8 @@
       <c r="IA2" s="1"/>
       <c r="IB2" s="1"/>
       <c r="IC2" s="1"/>
-      <c r="ID2" s="2"/>
       <c r="IE2" s="1"/>
       <c r="IF2" s="1"/>
-      <c r="IG2" s="2"/>
       <c r="IH2" s="1" t="s">
         <v>1</v>
       </c>
@@ -805,12 +729,10 @@
       <c r="IK2" s="1"/>
       <c r="IL2" s="1"/>
       <c r="IM2" s="1"/>
-      <c r="IN2" s="2"/>
       <c r="IO2" s="1"/>
       <c r="IP2" s="1"/>
-      <c r="IQ2" s="2"/>
-    </row>
-    <row r="3" spans="1:251">
+    </row>
+    <row r="3" spans="1:250">
       <c r="A3" s="1" t="inlineStr">
         <is>
           <t>Last modified: 2017/02/04</t>
@@ -825,7 +747,6 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="2"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -835,7 +756,6 @@
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
-      <c r="U3" s="2"/>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
@@ -845,7 +765,6 @@
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
-      <c r="AE3" s="2"/>
       <c r="AF3" s="1"/>
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
@@ -855,7 +774,6 @@
       <c r="AL3" s="1"/>
       <c r="AM3" s="1"/>
       <c r="AN3" s="1"/>
-      <c r="AO3" s="2"/>
       <c r="AP3" s="1"/>
       <c r="AQ3" s="1"/>
       <c r="AR3" s="1"/>
@@ -865,7 +783,6 @@
       <c r="AV3" s="1"/>
       <c r="AW3" s="1"/>
       <c r="AX3" s="1"/>
-      <c r="AY3" s="2"/>
       <c r="AZ3" s="1"/>
       <c r="BA3" s="1"/>
       <c r="BB3" s="1"/>
@@ -875,7 +792,6 @@
       <c r="BF3" s="1"/>
       <c r="BG3" s="1"/>
       <c r="BH3" s="1"/>
-      <c r="BI3" s="2"/>
       <c r="BJ3" s="1"/>
       <c r="BK3" s="1"/>
       <c r="BL3" s="1"/>
@@ -885,7 +801,6 @@
       <c r="BP3" s="1"/>
       <c r="BQ3" s="1"/>
       <c r="BR3" s="1"/>
-      <c r="BS3" s="2"/>
       <c r="BT3" s="1"/>
       <c r="BU3" s="1"/>
       <c r="BV3" s="1"/>
@@ -895,7 +810,6 @@
       <c r="BZ3" s="1"/>
       <c r="CA3" s="1"/>
       <c r="CB3" s="1"/>
-      <c r="CC3" s="2"/>
       <c r="CD3" s="1"/>
       <c r="CE3" s="1"/>
       <c r="CF3" s="1"/>
@@ -905,7 +819,6 @@
       <c r="CJ3" s="1"/>
       <c r="CK3" s="1"/>
       <c r="CL3" s="1"/>
-      <c r="CM3" s="2"/>
       <c r="CN3" s="1"/>
       <c r="CO3" s="1"/>
       <c r="CP3" s="1"/>
@@ -915,7 +828,6 @@
       <c r="CT3" s="1"/>
       <c r="CU3" s="1"/>
       <c r="CV3" s="1"/>
-      <c r="CW3" s="2"/>
       <c r="CX3" s="1"/>
       <c r="CY3" s="1"/>
       <c r="CZ3" s="1"/>
@@ -925,7 +837,6 @@
       <c r="DD3" s="1"/>
       <c r="DE3" s="1"/>
       <c r="DF3" s="1"/>
-      <c r="DG3" s="2"/>
       <c r="DH3" s="1"/>
       <c r="DI3" s="1"/>
       <c r="DJ3" s="1"/>
@@ -935,7 +846,6 @@
       <c r="DN3" s="1"/>
       <c r="DO3" s="1"/>
       <c r="DP3" s="1"/>
-      <c r="DQ3" s="2"/>
       <c r="DR3" s="1"/>
       <c r="DS3" s="1"/>
       <c r="DT3" s="1"/>
@@ -945,7 +855,6 @@
       <c r="DX3" s="1"/>
       <c r="DY3" s="1"/>
       <c r="DZ3" s="1"/>
-      <c r="EA3" s="2"/>
       <c r="EB3" s="1"/>
       <c r="EC3" s="1"/>
       <c r="ED3" s="1"/>
@@ -955,7 +864,6 @@
       <c r="EH3" s="1"/>
       <c r="EI3" s="1"/>
       <c r="EJ3" s="1"/>
-      <c r="EK3" s="2"/>
       <c r="EL3" s="1"/>
       <c r="EM3" s="1"/>
       <c r="EN3" s="1"/>
@@ -965,7 +873,6 @@
       <c r="ER3" s="1"/>
       <c r="ES3" s="1"/>
       <c r="ET3" s="1"/>
-      <c r="EU3" s="2"/>
       <c r="EV3" s="1"/>
       <c r="EW3" s="1"/>
       <c r="EX3" s="1"/>
@@ -975,7 +882,6 @@
       <c r="FB3" s="1"/>
       <c r="FC3" s="1"/>
       <c r="FD3" s="1"/>
-      <c r="FE3" s="2"/>
       <c r="FF3" s="1"/>
       <c r="FG3" s="1"/>
       <c r="FH3" s="1"/>
@@ -985,7 +891,6 @@
       <c r="FL3" s="1"/>
       <c r="FM3" s="1"/>
       <c r="FN3" s="1"/>
-      <c r="FO3" s="2"/>
       <c r="FP3" s="1"/>
       <c r="FQ3" s="1"/>
       <c r="FR3" s="1"/>
@@ -995,7 +900,6 @@
       <c r="FV3" s="1"/>
       <c r="FW3" s="1"/>
       <c r="FX3" s="1"/>
-      <c r="FY3" s="2"/>
       <c r="FZ3" s="1"/>
       <c r="GA3" s="1"/>
       <c r="GB3" s="1"/>
@@ -1005,7 +909,6 @@
       <c r="GF3" s="1"/>
       <c r="GG3" s="1"/>
       <c r="GH3" s="1"/>
-      <c r="GI3" s="2"/>
       <c r="GJ3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1017,7 +920,6 @@
       <c r="GP3" s="1"/>
       <c r="GQ3" s="1"/>
       <c r="GR3" s="1"/>
-      <c r="GS3" s="2"/>
       <c r="GT3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1029,7 +931,6 @@
       <c r="GZ3" s="1"/>
       <c r="HA3" s="1"/>
       <c r="HB3" s="1"/>
-      <c r="HC3" s="2"/>
       <c r="HD3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1041,7 +942,6 @@
       <c r="HJ3" s="1"/>
       <c r="HK3" s="1"/>
       <c r="HL3" s="1"/>
-      <c r="HM3" s="2"/>
       <c r="HN3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1053,7 +953,6 @@
       <c r="HT3" s="1"/>
       <c r="HU3" s="1"/>
       <c r="HV3" s="1"/>
-      <c r="HW3" s="2"/>
       <c r="HX3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1065,7 +964,6 @@
       <c r="ID3" s="1"/>
       <c r="IE3" s="1"/>
       <c r="IF3" s="1"/>
-      <c r="IG3" s="2"/>
       <c r="IH3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1077,9 +975,8 @@
       <c r="IN3" s="1"/>
       <c r="IO3" s="1"/>
       <c r="IP3" s="1"/>
-      <c r="IQ3" s="2"/>
-    </row>
-    <row r="4" spans="1:251">
+    </row>
+    <row r="4" spans="1:250">
       <c r="A4" s="1" t="inlineStr">
         <is>
           <t>PCB version: 1.0</t>
@@ -1094,7 +991,6 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="2"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -1104,7 +1000,6 @@
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
-      <c r="U4" s="2"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
@@ -1114,7 +1009,6 @@
       <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
-      <c r="AE4" s="2"/>
       <c r="AF4" s="1"/>
       <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
@@ -1124,7 +1018,6 @@
       <c r="AL4" s="1"/>
       <c r="AM4" s="1"/>
       <c r="AN4" s="1"/>
-      <c r="AO4" s="2"/>
       <c r="AP4" s="1"/>
       <c r="AQ4" s="1"/>
       <c r="AR4" s="1"/>
@@ -1134,7 +1027,6 @@
       <c r="AV4" s="1"/>
       <c r="AW4" s="1"/>
       <c r="AX4" s="1"/>
-      <c r="AY4" s="2"/>
       <c r="AZ4" s="1"/>
       <c r="BA4" s="1"/>
       <c r="BB4" s="1"/>
@@ -1144,7 +1036,6 @@
       <c r="BF4" s="1"/>
       <c r="BG4" s="1"/>
       <c r="BH4" s="1"/>
-      <c r="BI4" s="2"/>
       <c r="BJ4" s="1"/>
       <c r="BK4" s="1"/>
       <c r="BL4" s="1"/>
@@ -1154,7 +1045,6 @@
       <c r="BP4" s="1"/>
       <c r="BQ4" s="1"/>
       <c r="BR4" s="1"/>
-      <c r="BS4" s="2"/>
       <c r="BT4" s="1"/>
       <c r="BU4" s="1"/>
       <c r="BV4" s="1"/>
@@ -1164,7 +1054,6 @@
       <c r="BZ4" s="1"/>
       <c r="CA4" s="1"/>
       <c r="CB4" s="1"/>
-      <c r="CC4" s="2"/>
       <c r="CD4" s="1"/>
       <c r="CE4" s="1"/>
       <c r="CF4" s="1"/>
@@ -1174,7 +1063,6 @@
       <c r="CJ4" s="1"/>
       <c r="CK4" s="1"/>
       <c r="CL4" s="1"/>
-      <c r="CM4" s="2"/>
       <c r="CN4" s="1"/>
       <c r="CO4" s="1"/>
       <c r="CP4" s="1"/>
@@ -1184,7 +1072,6 @@
       <c r="CT4" s="1"/>
       <c r="CU4" s="1"/>
       <c r="CV4" s="1"/>
-      <c r="CW4" s="2"/>
       <c r="CX4" s="1"/>
       <c r="CY4" s="1"/>
       <c r="CZ4" s="1"/>
@@ -1194,7 +1081,6 @@
       <c r="DD4" s="1"/>
       <c r="DE4" s="1"/>
       <c r="DF4" s="1"/>
-      <c r="DG4" s="2"/>
       <c r="DH4" s="1"/>
       <c r="DI4" s="1"/>
       <c r="DJ4" s="1"/>
@@ -1204,7 +1090,6 @@
       <c r="DN4" s="1"/>
       <c r="DO4" s="1"/>
       <c r="DP4" s="1"/>
-      <c r="DQ4" s="2"/>
       <c r="DR4" s="1"/>
       <c r="DS4" s="1"/>
       <c r="DT4" s="1"/>
@@ -1214,7 +1099,6 @@
       <c r="DX4" s="1"/>
       <c r="DY4" s="1"/>
       <c r="DZ4" s="1"/>
-      <c r="EA4" s="2"/>
       <c r="EB4" s="1"/>
       <c r="EC4" s="1"/>
       <c r="ED4" s="1"/>
@@ -1224,7 +1108,6 @@
       <c r="EH4" s="1"/>
       <c r="EI4" s="1"/>
       <c r="EJ4" s="1"/>
-      <c r="EK4" s="2"/>
       <c r="EL4" s="1"/>
       <c r="EM4" s="1"/>
       <c r="EN4" s="1"/>
@@ -1234,7 +1117,6 @@
       <c r="ER4" s="1"/>
       <c r="ES4" s="1"/>
       <c r="ET4" s="1"/>
-      <c r="EU4" s="2"/>
       <c r="EV4" s="1"/>
       <c r="EW4" s="1"/>
       <c r="EX4" s="1"/>
@@ -1244,7 +1126,6 @@
       <c r="FB4" s="1"/>
       <c r="FC4" s="1"/>
       <c r="FD4" s="1"/>
-      <c r="FE4" s="2"/>
       <c r="FF4" s="1"/>
       <c r="FG4" s="1"/>
       <c r="FH4" s="1"/>
@@ -1254,7 +1135,6 @@
       <c r="FL4" s="1"/>
       <c r="FM4" s="1"/>
       <c r="FN4" s="1"/>
-      <c r="FO4" s="2"/>
       <c r="FP4" s="1"/>
       <c r="FQ4" s="1"/>
       <c r="FR4" s="1"/>
@@ -1264,7 +1144,6 @@
       <c r="FV4" s="1"/>
       <c r="FW4" s="1"/>
       <c r="FX4" s="1"/>
-      <c r="FY4" s="2"/>
       <c r="FZ4" s="1"/>
       <c r="GA4" s="1"/>
       <c r="GB4" s="1"/>
@@ -1274,7 +1153,6 @@
       <c r="GF4" s="1"/>
       <c r="GG4" s="1"/>
       <c r="GH4" s="1"/>
-      <c r="GI4" s="2"/>
       <c r="GJ4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1286,7 +1164,6 @@
       <c r="GP4" s="1"/>
       <c r="GQ4" s="1"/>
       <c r="GR4" s="1"/>
-      <c r="GS4" s="2"/>
       <c r="GT4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1298,7 +1175,6 @@
       <c r="GZ4" s="1"/>
       <c r="HA4" s="1"/>
       <c r="HB4" s="1"/>
-      <c r="HC4" s="2"/>
       <c r="HD4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1310,7 +1186,6 @@
       <c r="HJ4" s="1"/>
       <c r="HK4" s="1"/>
       <c r="HL4" s="1"/>
-      <c r="HM4" s="2"/>
       <c r="HN4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1322,7 +1197,6 @@
       <c r="HT4" s="1"/>
       <c r="HU4" s="1"/>
       <c r="HV4" s="1"/>
-      <c r="HW4" s="2"/>
       <c r="HX4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1334,7 +1208,6 @@
       <c r="ID4" s="1"/>
       <c r="IE4" s="1"/>
       <c r="IF4" s="1"/>
-      <c r="IG4" s="2"/>
       <c r="IH4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1346,9 +1219,8 @@
       <c r="IN4" s="1"/>
       <c r="IO4" s="1"/>
       <c r="IP4" s="1"/>
-      <c r="IQ4" s="2"/>
-    </row>
-    <row r="5" spans="1:251">
+    </row>
+    <row r="5" spans="1:250">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>BOM revision: 0</t>
@@ -1363,7 +1235,6 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-      <c r="K5" s="2"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -1373,7 +1244,6 @@
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
-      <c r="U5" s="2"/>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
@@ -1383,7 +1253,6 @@
       <c r="AB5" s="1"/>
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
-      <c r="AE5" s="2"/>
       <c r="AF5" s="1"/>
       <c r="AG5" s="1"/>
       <c r="AH5" s="1"/>
@@ -1393,7 +1262,6 @@
       <c r="AL5" s="1"/>
       <c r="AM5" s="1"/>
       <c r="AN5" s="1"/>
-      <c r="AO5" s="2"/>
       <c r="AP5" s="1"/>
       <c r="AQ5" s="1"/>
       <c r="AR5" s="1"/>
@@ -1403,7 +1271,6 @@
       <c r="AV5" s="1"/>
       <c r="AW5" s="1"/>
       <c r="AX5" s="1"/>
-      <c r="AY5" s="2"/>
       <c r="AZ5" s="1"/>
       <c r="BA5" s="1"/>
       <c r="BB5" s="1"/>
@@ -1413,7 +1280,6 @@
       <c r="BF5" s="1"/>
       <c r="BG5" s="1"/>
       <c r="BH5" s="1"/>
-      <c r="BI5" s="2"/>
       <c r="BJ5" s="1"/>
       <c r="BK5" s="1"/>
       <c r="BL5" s="1"/>
@@ -1423,7 +1289,6 @@
       <c r="BP5" s="1"/>
       <c r="BQ5" s="1"/>
       <c r="BR5" s="1"/>
-      <c r="BS5" s="2"/>
       <c r="BT5" s="1"/>
       <c r="BU5" s="1"/>
       <c r="BV5" s="1"/>
@@ -1433,7 +1298,6 @@
       <c r="BZ5" s="1"/>
       <c r="CA5" s="1"/>
       <c r="CB5" s="1"/>
-      <c r="CC5" s="2"/>
       <c r="CD5" s="1"/>
       <c r="CE5" s="1"/>
       <c r="CF5" s="1"/>
@@ -1443,7 +1307,6 @@
       <c r="CJ5" s="1"/>
       <c r="CK5" s="1"/>
       <c r="CL5" s="1"/>
-      <c r="CM5" s="2"/>
       <c r="CN5" s="1"/>
       <c r="CO5" s="1"/>
       <c r="CP5" s="1"/>
@@ -1453,7 +1316,6 @@
       <c r="CT5" s="1"/>
       <c r="CU5" s="1"/>
       <c r="CV5" s="1"/>
-      <c r="CW5" s="2"/>
       <c r="CX5" s="1"/>
       <c r="CY5" s="1"/>
       <c r="CZ5" s="1"/>
@@ -1463,7 +1325,6 @@
       <c r="DD5" s="1"/>
       <c r="DE5" s="1"/>
       <c r="DF5" s="1"/>
-      <c r="DG5" s="2"/>
       <c r="DH5" s="1"/>
       <c r="DI5" s="1"/>
       <c r="DJ5" s="1"/>
@@ -1473,7 +1334,6 @@
       <c r="DN5" s="1"/>
       <c r="DO5" s="1"/>
       <c r="DP5" s="1"/>
-      <c r="DQ5" s="2"/>
       <c r="DR5" s="1"/>
       <c r="DS5" s="1"/>
       <c r="DT5" s="1"/>
@@ -1483,7 +1343,6 @@
       <c r="DX5" s="1"/>
       <c r="DY5" s="1"/>
       <c r="DZ5" s="1"/>
-      <c r="EA5" s="2"/>
       <c r="EB5" s="1"/>
       <c r="EC5" s="1"/>
       <c r="ED5" s="1"/>
@@ -1493,7 +1352,6 @@
       <c r="EH5" s="1"/>
       <c r="EI5" s="1"/>
       <c r="EJ5" s="1"/>
-      <c r="EK5" s="2"/>
       <c r="EL5" s="1"/>
       <c r="EM5" s="1"/>
       <c r="EN5" s="1"/>
@@ -1503,7 +1361,6 @@
       <c r="ER5" s="1"/>
       <c r="ES5" s="1"/>
       <c r="ET5" s="1"/>
-      <c r="EU5" s="2"/>
       <c r="EV5" s="1"/>
       <c r="EW5" s="1"/>
       <c r="EX5" s="1"/>
@@ -1513,7 +1370,6 @@
       <c r="FB5" s="1"/>
       <c r="FC5" s="1"/>
       <c r="FD5" s="1"/>
-      <c r="FE5" s="2"/>
       <c r="FF5" s="1"/>
       <c r="FG5" s="1"/>
       <c r="FH5" s="1"/>
@@ -1523,7 +1379,6 @@
       <c r="FL5" s="1"/>
       <c r="FM5" s="1"/>
       <c r="FN5" s="1"/>
-      <c r="FO5" s="2"/>
       <c r="FP5" s="1"/>
       <c r="FQ5" s="1"/>
       <c r="FR5" s="1"/>
@@ -1533,7 +1388,6 @@
       <c r="FV5" s="1"/>
       <c r="FW5" s="1"/>
       <c r="FX5" s="1"/>
-      <c r="FY5" s="2"/>
       <c r="FZ5" s="1"/>
       <c r="GA5" s="1"/>
       <c r="GB5" s="1"/>
@@ -1543,7 +1397,6 @@
       <c r="GF5" s="1"/>
       <c r="GG5" s="1"/>
       <c r="GH5" s="1"/>
-      <c r="GI5" s="2"/>
       <c r="GJ5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1555,7 +1408,6 @@
       <c r="GP5" s="1"/>
       <c r="GQ5" s="1"/>
       <c r="GR5" s="1"/>
-      <c r="GS5" s="2"/>
       <c r="GT5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1567,7 +1419,6 @@
       <c r="GZ5" s="1"/>
       <c r="HA5" s="1"/>
       <c r="HB5" s="1"/>
-      <c r="HC5" s="2"/>
       <c r="HD5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1579,7 +1430,6 @@
       <c r="HJ5" s="1"/>
       <c r="HK5" s="1"/>
       <c r="HL5" s="1"/>
-      <c r="HM5" s="2"/>
       <c r="HN5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1591,7 +1441,6 @@
       <c r="HT5" s="1"/>
       <c r="HU5" s="1"/>
       <c r="HV5" s="1"/>
-      <c r="HW5" s="2"/>
       <c r="HX5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1603,7 +1452,6 @@
       <c r="ID5" s="1"/>
       <c r="IE5" s="1"/>
       <c r="IF5" s="1"/>
-      <c r="IG5" s="2"/>
       <c r="IH5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1615,9 +1463,8 @@
       <c r="IN5" s="1"/>
       <c r="IO5" s="1"/>
       <c r="IP5" s="1"/>
-      <c r="IQ5" s="2"/>
-    </row>
-    <row r="6" spans="1:251">
+    </row>
+    <row r="6" spans="1:250">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1628,7 +1475,6 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="2"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
@@ -1638,7 +1484,6 @@
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
-      <c r="U6" s="2"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
@@ -1648,7 +1493,6 @@
       <c r="AB6" s="1"/>
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
-      <c r="AE6" s="2"/>
       <c r="AF6" s="1"/>
       <c r="AG6" s="1"/>
       <c r="AH6" s="1"/>
@@ -1658,7 +1502,6 @@
       <c r="AL6" s="1"/>
       <c r="AM6" s="1"/>
       <c r="AN6" s="1"/>
-      <c r="AO6" s="2"/>
       <c r="AP6" s="1"/>
       <c r="AQ6" s="1"/>
       <c r="AR6" s="1"/>
@@ -1668,7 +1511,6 @@
       <c r="AV6" s="1"/>
       <c r="AW6" s="1"/>
       <c r="AX6" s="1"/>
-      <c r="AY6" s="2"/>
       <c r="AZ6" s="1"/>
       <c r="BA6" s="1"/>
       <c r="BB6" s="1"/>
@@ -1678,7 +1520,6 @@
       <c r="BF6" s="1"/>
       <c r="BG6" s="1"/>
       <c r="BH6" s="1"/>
-      <c r="BI6" s="2"/>
       <c r="BJ6" s="1"/>
       <c r="BK6" s="1"/>
       <c r="BL6" s="1"/>
@@ -1688,7 +1529,6 @@
       <c r="BP6" s="1"/>
       <c r="BQ6" s="1"/>
       <c r="BR6" s="1"/>
-      <c r="BS6" s="2"/>
       <c r="BT6" s="1"/>
       <c r="BU6" s="1"/>
       <c r="BV6" s="1"/>
@@ -1698,7 +1538,6 @@
       <c r="BZ6" s="1"/>
       <c r="CA6" s="1"/>
       <c r="CB6" s="1"/>
-      <c r="CC6" s="2"/>
       <c r="CD6" s="1"/>
       <c r="CE6" s="1"/>
       <c r="CF6" s="1"/>
@@ -1708,7 +1547,6 @@
       <c r="CJ6" s="1"/>
       <c r="CK6" s="1"/>
       <c r="CL6" s="1"/>
-      <c r="CM6" s="2"/>
       <c r="CN6" s="1"/>
       <c r="CO6" s="1"/>
       <c r="CP6" s="1"/>
@@ -1718,7 +1556,6 @@
       <c r="CT6" s="1"/>
       <c r="CU6" s="1"/>
       <c r="CV6" s="1"/>
-      <c r="CW6" s="2"/>
       <c r="CX6" s="1"/>
       <c r="CY6" s="1"/>
       <c r="CZ6" s="1"/>
@@ -1728,7 +1565,6 @@
       <c r="DD6" s="1"/>
       <c r="DE6" s="1"/>
       <c r="DF6" s="1"/>
-      <c r="DG6" s="2"/>
       <c r="DH6" s="1"/>
       <c r="DI6" s="1"/>
       <c r="DJ6" s="1"/>
@@ -1738,7 +1574,6 @@
       <c r="DN6" s="1"/>
       <c r="DO6" s="1"/>
       <c r="DP6" s="1"/>
-      <c r="DQ6" s="2"/>
       <c r="DR6" s="1"/>
       <c r="DS6" s="1"/>
       <c r="DT6" s="1"/>
@@ -1748,7 +1583,6 @@
       <c r="DX6" s="1"/>
       <c r="DY6" s="1"/>
       <c r="DZ6" s="1"/>
-      <c r="EA6" s="2"/>
       <c r="EB6" s="1"/>
       <c r="EC6" s="1"/>
       <c r="ED6" s="1"/>
@@ -1758,7 +1592,6 @@
       <c r="EH6" s="1"/>
       <c r="EI6" s="1"/>
       <c r="EJ6" s="1"/>
-      <c r="EK6" s="2"/>
       <c r="EL6" s="1"/>
       <c r="EM6" s="1"/>
       <c r="EN6" s="1"/>
@@ -1768,7 +1601,6 @@
       <c r="ER6" s="1"/>
       <c r="ES6" s="1"/>
       <c r="ET6" s="1"/>
-      <c r="EU6" s="2"/>
       <c r="EV6" s="1"/>
       <c r="EW6" s="1"/>
       <c r="EX6" s="1"/>
@@ -1778,7 +1610,6 @@
       <c r="FB6" s="1"/>
       <c r="FC6" s="1"/>
       <c r="FD6" s="1"/>
-      <c r="FE6" s="2"/>
       <c r="FF6" s="1"/>
       <c r="FG6" s="1"/>
       <c r="FH6" s="1"/>
@@ -1788,7 +1619,6 @@
       <c r="FL6" s="1"/>
       <c r="FM6" s="1"/>
       <c r="FN6" s="1"/>
-      <c r="FO6" s="2"/>
       <c r="FP6" s="1"/>
       <c r="FQ6" s="1"/>
       <c r="FR6" s="1"/>
@@ -1798,7 +1628,6 @@
       <c r="FV6" s="1"/>
       <c r="FW6" s="1"/>
       <c r="FX6" s="1"/>
-      <c r="FY6" s="2"/>
       <c r="FZ6" s="1"/>
       <c r="GA6" s="1"/>
       <c r="GB6" s="1"/>
@@ -1808,7 +1637,6 @@
       <c r="GF6" s="1"/>
       <c r="GG6" s="1"/>
       <c r="GH6" s="1"/>
-      <c r="GI6" s="2"/>
       <c r="GJ6" s="1"/>
       <c r="GK6" s="1"/>
       <c r="GL6" s="1"/>
@@ -1818,7 +1646,6 @@
       <c r="GP6" s="1"/>
       <c r="GQ6" s="1"/>
       <c r="GR6" s="1"/>
-      <c r="GS6" s="2"/>
       <c r="GT6" s="1"/>
       <c r="GU6" s="1"/>
       <c r="GV6" s="1"/>
@@ -1828,7 +1655,6 @@
       <c r="GZ6" s="1"/>
       <c r="HA6" s="1"/>
       <c r="HB6" s="1"/>
-      <c r="HC6" s="2"/>
       <c r="HD6" s="1"/>
       <c r="HE6" s="1"/>
       <c r="HF6" s="1"/>
@@ -1838,7 +1664,6 @@
       <c r="HJ6" s="1"/>
       <c r="HK6" s="1"/>
       <c r="HL6" s="1"/>
-      <c r="HM6" s="2"/>
       <c r="HN6" s="1"/>
       <c r="HO6" s="1"/>
       <c r="HP6" s="1"/>
@@ -1848,7 +1673,6 @@
       <c r="HT6" s="1"/>
       <c r="HU6" s="1"/>
       <c r="HV6" s="1"/>
-      <c r="HW6" s="2"/>
       <c r="HX6" s="1"/>
       <c r="HY6" s="1"/>
       <c r="HZ6" s="1"/>
@@ -1858,7 +1682,6 @@
       <c r="ID6" s="1"/>
       <c r="IE6" s="1"/>
       <c r="IF6" s="1"/>
-      <c r="IG6" s="2"/>
       <c r="IH6" s="1"/>
       <c r="II6" s="1"/>
       <c r="IJ6" s="1"/>
@@ -1868,9 +1691,8 @@
       <c r="IN6" s="1"/>
       <c r="IO6" s="1"/>
       <c r="IP6" s="1"/>
-      <c r="IQ6" s="2"/>
-    </row>
-    <row r="7" spans="1:251">
+    </row>
+    <row r="7" spans="1:250">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -2269,19 +2091,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:251">
-      <c r="A8" s="2">
+    <row r="8" spans="1:250">
+      <c r="A8">
         <v>2</v>
       </c>
-      <c r="B8" s="2" t="inlineStr">
+      <c r="B8" t="inlineStr">
         <is>
           <t>C11, C16</t>
         </is>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="2" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>CL05C200JB51PNC</t>
         </is>
@@ -2297,28 +2119,28 @@
       <c r="G8" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="2" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>1276-6601-1-ND</t>
         </is>
       </c>
     </row>
-    <row r="9" spans="1:251">
-      <c r="A9" s="2">
+    <row r="9" spans="1:250">
+      <c r="A9">
         <v>1</v>
       </c>
-      <c r="B9" s="2" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>C12</t>
         </is>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="2" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>CL05B472KA5VPNC</t>
         </is>
@@ -2334,28 +2156,28 @@
       <c r="G9" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" t="s">
         <v>18</v>
       </c>
-      <c r="I9" s="2" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>1276-6858-1-ND</t>
         </is>
       </c>
     </row>
-    <row r="10" spans="1:251">
-      <c r="A10" s="2">
+    <row r="10" spans="1:250">
+      <c r="A10">
         <v>1</v>
       </c>
-      <c r="B10" s="2" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>C13</t>
         </is>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="2" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>CL05A105KA5NQNC</t>
         </is>
@@ -2371,28 +2193,28 @@
       <c r="G10" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="2" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>1276-1445-1-ND</t>
         </is>
       </c>
     </row>
-    <row r="11" spans="1:251">
-      <c r="A11" s="2">
+    <row r="11" spans="1:250">
+      <c r="A11">
         <v>1</v>
       </c>
-      <c r="B11" s="2" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>C14</t>
         </is>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="2" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>CL10A226MP8NUNE</t>
         </is>
@@ -2408,30 +2230,30 @@
       <c r="G11" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" t="s">
         <v>18</v>
       </c>
-      <c r="I11" s="2" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>1276-1274-1-ND</t>
         </is>
       </c>
     </row>
-    <row r="12" spans="1:251">
-      <c r="A12" s="2">
+    <row r="12" spans="1:250">
+      <c r="A12">
         <v>8</v>
       </c>
-      <c r="B12" s="2" t="inlineStr">
+      <c r="B12" t="inlineStr">
         <is>
           <t>C1, C2, C4, C5, C7, C8, C10, C15</t>
         </is>
       </c>
-      <c r="C12" s="2" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>Murata</t>
         </is>
       </c>
-      <c r="D12" s="2" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>GRM31CR71A226KE15L</t>
         </is>
@@ -2447,59 +2269,65 @@
       <c r="G12" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" t="s">
         <v>18</v>
       </c>
-      <c r="I12" s="2" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>490-5309-1-ND</t>
         </is>
       </c>
     </row>
-    <row r="13" spans="1:251">
-      <c r="A13" s="2">
+    <row r="13" spans="1:250">
+      <c r="A13">
         <v>2</v>
       </c>
-      <c r="B13" s="2" t="inlineStr">
+      <c r="B13" t="inlineStr">
         <is>
           <t>C20, C21</t>
         </is>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>19</v>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>CL10A475KO8NNNC</t>
+        </is>
       </c>
       <c r="E13" t="s">
         <v>16</v>
       </c>
-      <c r="F13" t="s">
-        <v>20</v>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>4.7µF ±10% 16V Ceramic Capacitor X5R 0603 </t>
+        </is>
       </c>
       <c r="G13" t="s">
         <v>17</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" t="s">
         <v>18</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:251">
-      <c r="A14" s="2">
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>1276-1784-1-ND</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" spans="1:250">
+      <c r="A14">
         <v>10</v>
       </c>
-      <c r="B14" s="2" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>C3, C6, C9, C17, C18, C19, C22, C23, C24, C25</t>
         </is>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" t="s">
         <v>19</v>
       </c>
       <c r="E14" t="s">
@@ -2511,28 +2339,28 @@
       <c r="G14" t="s">
         <v>17</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" t="s">
         <v>18</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:251">
-      <c r="A15" s="2">
+    <row r="15" spans="1:250">
+      <c r="A15">
         <v>1</v>
       </c>
-      <c r="B15" s="2" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>CF1</t>
         </is>
       </c>
-      <c r="C15" s="2" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>Harting</t>
         </is>
       </c>
-      <c r="D15" s="2" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>15220122401000</t>
         </is>
@@ -2548,30 +2376,30 @@
       <c r="G15" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" t="s">
         <v>18</v>
       </c>
-      <c r="I15" s="2" t="inlineStr">
+      <c r="I15" t="inlineStr">
         <is>
           <t>1195-5663-1-ND</t>
         </is>
       </c>
     </row>
-    <row r="16" spans="1:251">
-      <c r="A16" s="2">
+    <row r="16" spans="1:250">
+      <c r="A16">
         <v>1</v>
       </c>
-      <c r="B16" s="2" t="inlineStr">
+      <c r="B16" t="inlineStr">
         <is>
           <t>CF2</t>
         </is>
       </c>
-      <c r="C16" s="2" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>PreciDip</t>
         </is>
       </c>
-      <c r="D16" s="2" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>831-87-050-40-001101</t>
         </is>
@@ -2587,30 +2415,30 @@
       <c r="G16" t="s">
         <v>22</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" t="s">
         <v>18</v>
       </c>
-      <c r="I16" s="2" t="inlineStr">
+      <c r="I16" t="inlineStr">
         <is>
           <t>1212-1893-ND</t>
         </is>
       </c>
     </row>
-    <row r="17" spans="1:251">
-      <c r="A17" s="2">
+    <row r="17" spans="1:250">
+      <c r="A17">
         <v>2</v>
       </c>
-      <c r="B17" s="2" t="inlineStr">
+      <c r="B17" t="inlineStr">
         <is>
           <t>D1, D3</t>
         </is>
       </c>
-      <c r="C17" s="2" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>ST</t>
         </is>
       </c>
-      <c r="D17" s="2" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>STPS1L40AY</t>
         </is>
@@ -2626,30 +2454,30 @@
       <c r="G17" t="s">
         <v>22</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" t="s">
         <v>18</v>
       </c>
-      <c r="I17" s="2" t="inlineStr">
+      <c r="I17" t="inlineStr">
         <is>
           <t>497-12286-1-ND</t>
         </is>
       </c>
     </row>
-    <row r="18" spans="1:251">
-      <c r="A18" s="2">
+    <row r="18" spans="1:250">
+      <c r="A18">
         <v>1</v>
       </c>
-      <c r="B18" s="2" t="inlineStr">
+      <c r="B18" t="inlineStr">
         <is>
           <t>D2</t>
         </is>
       </c>
-      <c r="C18" s="2" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>Vishay</t>
         </is>
       </c>
-      <c r="D18" s="2" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>P4SMA6.8A-E3/61</t>
         </is>
@@ -2665,30 +2493,30 @@
       <c r="G18" t="s">
         <v>22</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" t="s">
         <v>18</v>
       </c>
-      <c r="I18" s="2" t="inlineStr">
+      <c r="I18" t="inlineStr">
         <is>
           <t>P4SMA6.8A-E3/61GICT-ND</t>
         </is>
       </c>
     </row>
-    <row r="19" spans="1:251">
-      <c r="A19" s="2">
+    <row r="19" spans="1:250">
+      <c r="A19">
         <v>1</v>
       </c>
-      <c r="B19" s="2" t="inlineStr">
+      <c r="B19" t="inlineStr">
         <is>
           <t>L1</t>
         </is>
       </c>
-      <c r="C19" s="2" t="inlineStr">
+      <c r="C19" t="inlineStr">
         <is>
           <t>Taiyo Yuden</t>
         </is>
       </c>
-      <c r="D19" s="2" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>CB2012T100KR</t>
         </is>
@@ -2704,28 +2532,28 @@
       <c r="G19" t="s">
         <v>22</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H19" t="s">
         <v>18</v>
       </c>
-      <c r="I19" s="2" t="inlineStr">
+      <c r="I19" t="inlineStr">
         <is>
           <t>587-2452-1-ND</t>
         </is>
       </c>
     </row>
-    <row r="20" spans="1:251">
-      <c r="A20" s="2">
+    <row r="20" spans="1:250">
+      <c r="A20">
         <v>1</v>
       </c>
-      <c r="B20" s="2" t="inlineStr">
+      <c r="B20" t="inlineStr">
         <is>
           <t>L2</t>
         </is>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="2" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>IFSC1515AHER220M01</t>
         </is>
@@ -2741,32 +2569,32 @@
       <c r="G20" t="s">
         <v>22</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="H20" t="s">
         <v>18</v>
       </c>
-      <c r="I20" s="2" t="inlineStr">
+      <c r="I20" t="inlineStr">
         <is>
           <t>541-1407-1-ND</t>
         </is>
       </c>
     </row>
-    <row r="21" spans="1:251">
-      <c r="A21" s="2">
+    <row r="21" spans="1:250">
+      <c r="A21">
         <v>1</v>
       </c>
-      <c r="B21" s="2" t="inlineStr">
+      <c r="B21" t="inlineStr">
         <is>
           <t>Q1</t>
         </is>
       </c>
-      <c r="C21" s="2" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>ON Semiconductor</t>
         </is>
       </c>
-      <c r="D21" s="2" t="inlineStr">
-        <is>
-          <t>2N7002WT1G</t>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>2N7002ET1G</t>
         </is>
       </c>
       <c r="E21" t="s">
@@ -2774,36 +2602,36 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>N-Channel 60V 310mA (Ta) 280mW (Tj) Surface Mount SC-70-3 (SOT323)</t>
+          <t>N-Channel 60V 260mA (Ta) 300mW (Tj) Surface Mount SOT-23-3 (TO-236)</t>
         </is>
       </c>
       <c r="G21" t="s">
         <v>22</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H21" t="s">
         <v>18</v>
       </c>
-      <c r="I21" s="2" t="inlineStr">
-        <is>
-          <t>2N7002WT1GOSCT-ND</t>
-        </is>
-      </c>
-    </row>
-    <row r="22" spans="1:251">
-      <c r="A22" s="2">
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>2N7002ET1GOSCT-ND</t>
+        </is>
+      </c>
+    </row>
+    <row r="22" spans="1:250">
+      <c r="A22">
         <v>1</v>
       </c>
-      <c r="B22" s="2" t="inlineStr">
+      <c r="B22" t="inlineStr">
         <is>
           <t>Q2</t>
         </is>
       </c>
-      <c r="C22" s="2" t="inlineStr">
+      <c r="C22" t="inlineStr">
         <is>
           <t>Vishay Siliconix</t>
         </is>
       </c>
-      <c r="D22" s="2" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>SI4431CDY-T1-GE3</t>
         </is>
@@ -2819,30 +2647,30 @@
       <c r="G22" t="s">
         <v>22</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="H22" t="s">
         <v>18</v>
       </c>
-      <c r="I22" s="2" t="inlineStr">
+      <c r="I22" t="inlineStr">
         <is>
           <t>SI4431CDY-T1-GE3CT-ND</t>
         </is>
       </c>
     </row>
-    <row r="23" spans="1:251">
-      <c r="A23" s="2">
+    <row r="23" spans="1:250">
+      <c r="A23">
         <v>1</v>
       </c>
-      <c r="B23" s="2" t="inlineStr">
+      <c r="B23" t="inlineStr">
         <is>
           <t>Q3</t>
         </is>
       </c>
-      <c r="C23" s="2" t="inlineStr">
+      <c r="C23" t="inlineStr">
         <is>
           <t>Fairchild/ON Semiconductor</t>
         </is>
       </c>
-      <c r="D23" s="2" t="inlineStr">
+      <c r="D23" t="inlineStr">
         <is>
           <t>MMBT3904</t>
         </is>
@@ -2858,28 +2686,28 @@
       <c r="G23" t="s">
         <v>22</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="H23" t="s">
         <v>18</v>
       </c>
-      <c r="I23" s="2" t="inlineStr">
+      <c r="I23" t="inlineStr">
         <is>
           <t>MMBT3904FSCT-ND</t>
         </is>
       </c>
     </row>
-    <row r="24" spans="1:251">
-      <c r="A24" s="2">
+    <row r="24" spans="1:250">
+      <c r="A24">
         <v>1</v>
       </c>
-      <c r="B24" s="2" t="inlineStr">
+      <c r="B24" t="inlineStr">
         <is>
           <t>R11</t>
         </is>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" t="s">
         <v>25</v>
       </c>
       <c r="E24" t="inlineStr">
@@ -2893,26 +2721,26 @@
       <c r="G24" t="s">
         <v>17</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="H24" t="s">
         <v>18</v>
       </c>
-      <c r="I24" s="2" t="s">
+      <c r="I24" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:251">
-      <c r="A25" s="2">
+    <row r="25" spans="1:250">
+      <c r="A25">
         <v>1</v>
       </c>
-      <c r="B25" s="2" t="inlineStr">
+      <c r="B25" t="inlineStr">
         <is>
           <t>R13</t>
         </is>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="2" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>RC1005F6653CS</t>
         </is>
@@ -2928,28 +2756,28 @@
       <c r="G25" t="s">
         <v>17</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="H25" t="s">
         <v>18</v>
       </c>
-      <c r="I25" s="2" t="inlineStr">
+      <c r="I25" t="inlineStr">
         <is>
           <t>1276-4275-1-ND</t>
         </is>
       </c>
     </row>
-    <row r="26" spans="1:251">
-      <c r="A26" s="2">
+    <row r="26" spans="1:250">
+      <c r="A26">
         <v>1</v>
       </c>
-      <c r="B26" s="2" t="inlineStr">
+      <c r="B26" t="inlineStr">
         <is>
           <t>R14</t>
         </is>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="2" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t>RC1005F3323CS</t>
         </is>
@@ -2965,28 +2793,28 @@
       <c r="G26" t="s">
         <v>17</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="H26" t="s">
         <v>18</v>
       </c>
-      <c r="I26" s="2" t="inlineStr">
+      <c r="I26" t="inlineStr">
         <is>
           <t>1276-4245-1-ND</t>
         </is>
       </c>
     </row>
-    <row r="27" spans="1:251">
-      <c r="A27" s="2">
+    <row r="27" spans="1:250">
+      <c r="A27">
         <v>1</v>
       </c>
-      <c r="B27" s="2" t="inlineStr">
+      <c r="B27" t="inlineStr">
         <is>
           <t>R15</t>
         </is>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" t="s">
         <v>25</v>
       </c>
       <c r="E27" t="s">
@@ -2998,26 +2826,26 @@
       <c r="G27" t="s">
         <v>17</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="H27" t="s">
         <v>18</v>
       </c>
-      <c r="I27" s="2" t="s">
+      <c r="I27" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:251">
-      <c r="A28" s="2">
+    <row r="28" spans="1:250">
+      <c r="A28">
         <v>1</v>
       </c>
-      <c r="B28" s="2" t="inlineStr">
+      <c r="B28" t="inlineStr">
         <is>
           <t>R16</t>
         </is>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="2" t="inlineStr">
+      <c r="D28" t="inlineStr">
         <is>
           <t>MCR01MZPJ000</t>
         </is>
@@ -3033,28 +2861,28 @@
       <c r="G28" t="s">
         <v>17</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="H28" t="s">
         <v>18</v>
       </c>
-      <c r="I28" s="2" t="inlineStr">
+      <c r="I28" t="inlineStr">
         <is>
           <t>RHM0.0JCT-ND</t>
         </is>
       </c>
     </row>
-    <row r="29" spans="1:251">
-      <c r="A29" s="2">
+    <row r="29" spans="1:250">
+      <c r="A29">
         <v>3</v>
       </c>
-      <c r="B29" s="2" t="inlineStr">
+      <c r="B29" t="inlineStr">
         <is>
           <t>R1, R10, R12</t>
         </is>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="2" t="inlineStr">
+      <c r="D29" t="inlineStr">
         <is>
           <t>MCR01MZPF1002</t>
         </is>
@@ -3070,28 +2898,28 @@
       <c r="G29" t="s">
         <v>17</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="H29" t="s">
         <v>18</v>
       </c>
-      <c r="I29" s="2" t="inlineStr">
+      <c r="I29" t="inlineStr">
         <is>
           <t>RHM10.0KLCT-ND</t>
         </is>
       </c>
     </row>
-    <row r="30" spans="1:251">
-      <c r="A30" s="2">
+    <row r="30" spans="1:250">
+      <c r="A30">
         <v>1</v>
       </c>
-      <c r="B30" s="2" t="inlineStr">
+      <c r="B30" t="inlineStr">
         <is>
           <t>R2</t>
         </is>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="2" t="inlineStr">
+      <c r="D30" t="inlineStr">
         <is>
           <t>MCR01MRTF1003</t>
         </is>
@@ -3107,28 +2935,28 @@
       <c r="G30" t="s">
         <v>17</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="H30" t="s">
         <v>18</v>
       </c>
-      <c r="I30" s="2" t="inlineStr">
+      <c r="I30" t="inlineStr">
         <is>
           <t>RHM100KCDCT-ND</t>
         </is>
       </c>
     </row>
-    <row r="31" spans="1:251">
-      <c r="A31" s="2">
+    <row r="31" spans="1:250">
+      <c r="A31">
         <v>2</v>
       </c>
-      <c r="B31" s="2" t="inlineStr">
+      <c r="B31" t="inlineStr">
         <is>
           <t>R22, R23</t>
         </is>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="2" t="inlineStr">
+      <c r="D31" t="inlineStr">
         <is>
           <t>TRR01MZPF4701</t>
         </is>
@@ -3144,28 +2972,28 @@
       <c r="G31" t="s">
         <v>17</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="H31" t="s">
         <v>18</v>
       </c>
-      <c r="I31" s="2" t="inlineStr">
+      <c r="I31" t="inlineStr">
         <is>
           <t>RHM4.7KBHCT-ND</t>
         </is>
       </c>
     </row>
-    <row r="32" spans="1:251">
-      <c r="A32" s="2">
+    <row r="32" spans="1:250">
+      <c r="A32">
         <v>3</v>
       </c>
-      <c r="B32" s="2" t="inlineStr">
+      <c r="B32" t="inlineStr">
         <is>
           <t>R3, R4, R5</t>
         </is>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" t="s">
         <v>24</v>
       </c>
-      <c r="D32" s="2" t="inlineStr">
+      <c r="D32" t="inlineStr">
         <is>
           <t>MCR01MZPF1001</t>
         </is>
@@ -3181,28 +3009,28 @@
       <c r="G32" t="s">
         <v>17</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="H32" t="s">
         <v>18</v>
       </c>
-      <c r="I32" s="2" t="inlineStr">
+      <c r="I32" t="inlineStr">
         <is>
           <t>RHM1.00KLCT-ND</t>
         </is>
       </c>
     </row>
-    <row r="33" spans="1:251">
-      <c r="A33" s="2">
+    <row r="33" spans="1:250">
+      <c r="A33">
         <v>2</v>
       </c>
-      <c r="B33" s="2" t="inlineStr">
+      <c r="B33" t="inlineStr">
         <is>
           <t>R6, R9</t>
         </is>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" t="s">
         <v>23</v>
       </c>
-      <c r="D33" s="2" t="inlineStr">
+      <c r="D33" t="inlineStr">
         <is>
           <t>RCWE0805R180FKEA</t>
         </is>
@@ -3218,28 +3046,28 @@
       <c r="G33" t="s">
         <v>17</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="H33" t="s">
         <v>18</v>
       </c>
-      <c r="I33" s="2" t="inlineStr">
+      <c r="I33" t="inlineStr">
         <is>
           <t>541-2730-1-ND</t>
         </is>
       </c>
     </row>
-    <row r="34" spans="1:251">
-      <c r="A34" s="2">
+    <row r="34" spans="1:250">
+      <c r="A34">
         <v>1</v>
       </c>
-      <c r="B34" s="2" t="inlineStr">
+      <c r="B34" t="inlineStr">
         <is>
           <t>R7</t>
         </is>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" t="s">
         <v>15</v>
       </c>
-      <c r="D34" s="2" t="inlineStr">
+      <c r="D34" t="inlineStr">
         <is>
           <t>RC1005F8663CS</t>
         </is>
@@ -3255,28 +3083,28 @@
       <c r="G34" t="s">
         <v>17</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="H34" t="s">
         <v>18</v>
       </c>
-      <c r="I34" s="2" t="inlineStr">
+      <c r="I34" t="inlineStr">
         <is>
           <t>1276-4285-1-ND</t>
         </is>
       </c>
     </row>
-    <row r="35" spans="1:251">
-      <c r="A35" s="2">
+    <row r="35" spans="1:250">
+      <c r="A35">
         <v>1</v>
       </c>
-      <c r="B35" s="2" t="inlineStr">
+      <c r="B35" t="inlineStr">
         <is>
           <t>R8</t>
         </is>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="2" t="inlineStr">
+      <c r="D35" t="inlineStr">
         <is>
           <t>CRCW0402274KFKED</t>
         </is>
@@ -3292,28 +3120,28 @@
       <c r="G35" t="s">
         <v>17</v>
       </c>
-      <c r="H35" s="2" t="s">
+      <c r="H35" t="s">
         <v>18</v>
       </c>
-      <c r="I35" s="2" t="inlineStr">
+      <c r="I35" t="inlineStr">
         <is>
           <t>541-274KLCT-ND</t>
         </is>
       </c>
     </row>
-    <row r="36" spans="1:251">
-      <c r="A36" s="2">
+    <row r="36" spans="1:250">
+      <c r="A36">
         <v>1</v>
       </c>
-      <c r="B36" s="2" t="inlineStr">
+      <c r="B36" t="inlineStr">
         <is>
           <t>U1</t>
         </is>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" t="s">
         <v>29</v>
       </c>
-      <c r="D36" s="2" t="inlineStr">
+      <c r="D36" t="inlineStr">
         <is>
           <t>SPV1040T</t>
         </is>
@@ -3329,30 +3157,30 @@
       <c r="G36" t="s">
         <v>22</v>
       </c>
-      <c r="H36" s="2" t="s">
+      <c r="H36" t="s">
         <v>18</v>
       </c>
-      <c r="I36" s="2" t="inlineStr">
+      <c r="I36" t="inlineStr">
         <is>
           <t>497-11417-ND</t>
         </is>
       </c>
     </row>
-    <row r="37" spans="1:251">
-      <c r="A37" s="2">
+    <row r="37" spans="1:250">
+      <c r="A37">
         <v>1</v>
       </c>
-      <c r="B37" s="2" t="inlineStr">
+      <c r="B37" t="inlineStr">
         <is>
           <t>U2</t>
         </is>
       </c>
-      <c r="C37" s="2" t="inlineStr">
+      <c r="C37" t="inlineStr">
         <is>
           <t>Texas Instruments</t>
         </is>
       </c>
-      <c r="D37" s="2" t="inlineStr">
+      <c r="D37" t="inlineStr">
         <is>
           <t>TCAN330GDCNT</t>
         </is>
@@ -3368,30 +3196,30 @@
       <c r="G37" t="s">
         <v>22</v>
       </c>
-      <c r="H37" s="2" t="s">
+      <c r="H37" t="s">
         <v>18</v>
       </c>
-      <c r="I37" s="2" t="inlineStr">
+      <c r="I37" t="inlineStr">
         <is>
           <t>296-44211-1-ND</t>
         </is>
       </c>
     </row>
-    <row r="38" spans="1:251">
-      <c r="A38" s="2">
+    <row r="38" spans="1:250">
+      <c r="A38">
         <v>1</v>
       </c>
-      <c r="B38" s="2" t="inlineStr">
+      <c r="B38" t="inlineStr">
         <is>
           <t>U3</t>
         </is>
       </c>
-      <c r="C38" s="2" t="inlineStr">
+      <c r="C38" t="inlineStr">
         <is>
           <t>TI</t>
         </is>
       </c>
-      <c r="D38" s="2" t="inlineStr">
+      <c r="D38" t="inlineStr">
         <is>
           <t>LM3671MF-3.3/NOPB</t>
         </is>
@@ -3407,30 +3235,30 @@
       <c r="G38" t="s">
         <v>22</v>
       </c>
-      <c r="H38" s="2" t="s">
+      <c r="H38" t="s">
         <v>18</v>
       </c>
-      <c r="I38" s="2" t="inlineStr">
+      <c r="I38" t="inlineStr">
         <is>
           <t>LM3671MF-3.3/NOPBCT-ND</t>
         </is>
       </c>
     </row>
-    <row r="39" spans="1:251">
-      <c r="A39" s="2">
+    <row r="39" spans="1:250">
+      <c r="A39">
         <v>1</v>
       </c>
-      <c r="B39" s="2" t="inlineStr">
+      <c r="B39" t="inlineStr">
         <is>
           <t>U5</t>
         </is>
       </c>
-      <c r="C39" s="2" t="inlineStr">
+      <c r="C39" t="inlineStr">
         <is>
           <t>Linear Technology</t>
         </is>
       </c>
-      <c r="D39" s="2" t="inlineStr">
+      <c r="D39" t="inlineStr">
         <is>
           <t>LTC2990CMS#PBF</t>
         </is>
@@ -3446,28 +3274,28 @@
       <c r="G39" t="s">
         <v>22</v>
       </c>
-      <c r="H39" s="2" t="s">
+      <c r="H39" t="s">
         <v>18</v>
       </c>
-      <c r="I39" s="2" t="inlineStr">
+      <c r="I39" t="inlineStr">
         <is>
           <t>LTC2990CMS#PBF-ND</t>
         </is>
       </c>
     </row>
-    <row r="40" spans="1:251">
-      <c r="A40" s="2">
+    <row r="40" spans="1:250">
+      <c r="A40">
         <v>1</v>
       </c>
-      <c r="B40" s="2" t="inlineStr">
+      <c r="B40" t="inlineStr">
         <is>
           <t>U6</t>
         </is>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" t="s">
         <v>29</v>
       </c>
-      <c r="D40" s="2" t="inlineStr">
+      <c r="D40" t="inlineStr">
         <is>
           <t>STM32F042K6T6</t>
         </is>
@@ -3483,30 +3311,30 @@
       <c r="G40" t="s">
         <v>22</v>
       </c>
-      <c r="H40" s="2" t="s">
+      <c r="H40" t="s">
         <v>18</v>
       </c>
-      <c r="I40" s="2" t="inlineStr">
+      <c r="I40" t="inlineStr">
         <is>
           <t>497-14647-ND</t>
         </is>
       </c>
     </row>
-    <row r="41" spans="1:251">
-      <c r="A41" s="2">
+    <row r="41" spans="1:250">
+      <c r="A41">
         <v>1</v>
       </c>
-      <c r="B41" s="2" t="inlineStr">
+      <c r="B41" t="inlineStr">
         <is>
           <t>X1</t>
         </is>
       </c>
-      <c r="C41" s="2" t="inlineStr">
+      <c r="C41" t="inlineStr">
         <is>
           <t>ECS Inc.</t>
         </is>
       </c>
-      <c r="D41" s="2" t="inlineStr">
+      <c r="D41" t="inlineStr">
         <is>
           <t>ECS-80-18-20BQ-DS</t>
         </is>
@@ -3522,231 +3350,184 @@
       <c r="G41" t="s">
         <v>22</v>
       </c>
-      <c r="H41" s="2" t="s">
+      <c r="H41" t="s">
         <v>18</v>
       </c>
-      <c r="I41" s="2" t="inlineStr">
+      <c r="I41" t="inlineStr">
         <is>
           <t>XC2015CT-ND</t>
         </is>
       </c>
     </row>
-    <row r="42" spans="1:251">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-    </row>
-    <row r="50" spans="1:251">
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="2"/>
-    </row>
-    <row r="51" spans="1:251">
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="2"/>
-    </row>
-    <row r="52" spans="1:251">
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="2"/>
-    </row>
-    <row r="53" spans="1:251">
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="2"/>
-    </row>
-    <row r="54" spans="1:251">
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="2"/>
-    </row>
-    <row r="55" spans="1:251">
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="2"/>
-    </row>
-    <row r="56" spans="1:251">
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
-      <c r="G56" s="2"/>
-    </row>
-    <row r="57" spans="1:251">
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
-      <c r="G57" s="2"/>
-    </row>
-    <row r="58" spans="1:251">
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
-      <c r="G58" s="2"/>
-    </row>
-    <row r="59" spans="1:251">
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3"/>
-      <c r="G59" s="2"/>
-    </row>
-    <row r="60" spans="1:251">
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3"/>
-      <c r="G60" s="2"/>
-    </row>
-    <row r="61" spans="1:251">
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
-      <c r="G61" s="2"/>
-    </row>
-    <row r="62" spans="1:251">
-      <c r="D62" s="3"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="3"/>
-      <c r="G62" s="2"/>
-    </row>
-    <row r="63" spans="1:251">
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-      <c r="G63" s="2"/>
-    </row>
-    <row r="64" spans="1:251">
-      <c r="D64" s="3"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
-      <c r="G64" s="2"/>
-    </row>
-    <row r="65" spans="1:251">
-      <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3"/>
-      <c r="G65" s="2"/>
-    </row>
-    <row r="66" spans="1:251">
-      <c r="D66" s="3"/>
-      <c r="E66" s="3"/>
-      <c r="F66" s="3"/>
-      <c r="G66" s="2"/>
-    </row>
-    <row r="67" spans="1:251">
-      <c r="D67" s="3"/>
-      <c r="E67" s="3"/>
-      <c r="F67" s="3"/>
-      <c r="G67" s="2"/>
-    </row>
-    <row r="68" spans="1:251">
-      <c r="D68" s="3"/>
-      <c r="E68" s="3"/>
-      <c r="F68" s="3"/>
-      <c r="G68" s="2"/>
-    </row>
-    <row r="69" spans="1:251">
-      <c r="D69" s="3"/>
-      <c r="E69" s="3"/>
-      <c r="F69" s="3"/>
-      <c r="G69" s="2"/>
-    </row>
-    <row r="70" spans="1:251">
-      <c r="D70" s="3"/>
-      <c r="E70" s="3"/>
-      <c r="F70" s="3"/>
-      <c r="G70" s="2"/>
-    </row>
-    <row r="71" spans="1:251">
-      <c r="D71" s="3"/>
-      <c r="E71" s="3"/>
-      <c r="F71" s="3"/>
-      <c r="G71" s="2"/>
-    </row>
-    <row r="72" spans="1:251">
-      <c r="D72" s="3"/>
-      <c r="E72" s="3"/>
-      <c r="F72" s="3"/>
-      <c r="G72" s="2"/>
-    </row>
-    <row r="73" spans="1:251">
-      <c r="D73" s="3"/>
-      <c r="E73" s="3"/>
-      <c r="F73" s="3"/>
-      <c r="G73" s="2"/>
-    </row>
-    <row r="74" spans="1:251">
-      <c r="D74" s="3"/>
-      <c r="E74" s="3"/>
-      <c r="F74" s="3"/>
-      <c r="G74" s="2"/>
-    </row>
-    <row r="75" spans="1:251">
-      <c r="D75" s="3"/>
-      <c r="E75" s="3"/>
-      <c r="F75" s="3"/>
-      <c r="G75" s="2"/>
-    </row>
-    <row r="76" spans="1:251">
-      <c r="D76" s="3"/>
-      <c r="E76" s="3"/>
-      <c r="F76" s="3"/>
-      <c r="G76" s="2"/>
-    </row>
-    <row r="77" spans="1:251">
-      <c r="D77" s="3"/>
-      <c r="E77" s="3"/>
-      <c r="F77" s="3"/>
-      <c r="G77" s="2"/>
-    </row>
-    <row r="78" spans="1:251">
-      <c r="D78" s="3"/>
-      <c r="E78" s="3"/>
-      <c r="F78" s="3"/>
-      <c r="G78" s="2"/>
-    </row>
-    <row r="79" spans="1:251">
-      <c r="D79" s="3"/>
-      <c r="E79" s="3"/>
-      <c r="F79" s="3"/>
-      <c r="G79" s="2"/>
-    </row>
-    <row r="80" spans="1:251">
-      <c r="D80" s="3"/>
-      <c r="E80" s="3"/>
-      <c r="F80" s="3"/>
-      <c r="G80" s="2"/>
-    </row>
-    <row r="81" spans="1:251">
-      <c r="D81" s="3"/>
-      <c r="E81" s="3"/>
-      <c r="F81" s="3"/>
-      <c r="G81" s="2"/>
-    </row>
-    <row r="82" spans="1:251">
-      <c r="D82" s="3"/>
-      <c r="E82" s="3"/>
-      <c r="F82" s="3"/>
-      <c r="G82" s="2"/>
-    </row>
-    <row r="83" spans="1:251">
-      <c r="D83" s="3"/>
-      <c r="E83" s="3"/>
-      <c r="F83" s="3"/>
-      <c r="G83" s="2"/>
+    <row r="50" spans="1:250">
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+    </row>
+    <row r="51" spans="1:250">
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+    </row>
+    <row r="52" spans="1:250">
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+    </row>
+    <row r="53" spans="1:250">
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+    </row>
+    <row r="54" spans="1:250">
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+    </row>
+    <row r="55" spans="1:250">
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+    </row>
+    <row r="56" spans="1:250">
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+    </row>
+    <row r="57" spans="1:250">
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+    </row>
+    <row r="58" spans="1:250">
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+    </row>
+    <row r="59" spans="1:250">
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+    </row>
+    <row r="60" spans="1:250">
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+    </row>
+    <row r="61" spans="1:250">
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+    </row>
+    <row r="62" spans="1:250">
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+    </row>
+    <row r="63" spans="1:250">
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+    </row>
+    <row r="64" spans="1:250">
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+    </row>
+    <row r="65" spans="1:250">
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+    </row>
+    <row r="66" spans="1:250">
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+    </row>
+    <row r="67" spans="1:250">
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+    </row>
+    <row r="68" spans="1:250">
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+    </row>
+    <row r="69" spans="1:250">
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+    </row>
+    <row r="70" spans="1:250">
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+    </row>
+    <row r="71" spans="1:250">
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+    </row>
+    <row r="72" spans="1:250">
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+    </row>
+    <row r="73" spans="1:250">
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+    </row>
+    <row r="74" spans="1:250">
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+    </row>
+    <row r="75" spans="1:250">
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+    </row>
+    <row r="76" spans="1:250">
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+    </row>
+    <row r="77" spans="1:250">
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
+    </row>
+    <row r="78" spans="1:250">
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+    </row>
+    <row r="79" spans="1:250">
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+    </row>
+    <row r="80" spans="1:250">
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+    </row>
+    <row r="81" spans="1:250">
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+    </row>
+    <row r="82" spans="1:250">
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+    </row>
+    <row r="83" spans="1:250">
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>

</xml_diff>